<commit_message>
finished work in 1980s 1990s
finished 1980s and 1990s, then did variable analysis on total variables to be used in data study. some need renaming: I'll have to clone the datasets to get that. I still have to build data tables based on year, anyway, but during this I can rename column headings so they're consistent. We could talk about this, as i don't really have to rename them now that i know what code they are listed under. In Tableau we can rename them there anyway if we want.
</commit_message>
<xml_diff>
--- a/variable selection program.xlsx
+++ b/variable selection program.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.creznic/Documents/GitHub/ProjectVatican-II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFB1B6D-6AC2-B44D-8406-E288288C412F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C722F13-281B-A248-90B6-BD38D71732A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0A937964-CD54-FA4F-B1E1-727FE8EF5B80}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
   <si>
     <t xml:space="preserve">Square Miles, 1960 (SQMILE60) </t>
   </si>
@@ -322,12 +323,123 @@
   <si>
     <t>STTLNF70</t>
   </si>
+  <si>
+    <t>SLD8001</t>
+  </si>
+  <si>
+    <t>ELEM80</t>
+  </si>
+  <si>
+    <t>TELEM80</t>
+  </si>
+  <si>
+    <t>LAYEL80</t>
+  </si>
+  <si>
+    <t>SSA80</t>
+  </si>
+  <si>
+    <t>SEC80</t>
+  </si>
+  <si>
+    <t>TSEC80</t>
+  </si>
+  <si>
+    <t>LAYSEC80</t>
+  </si>
+  <si>
+    <t>ACASCH80</t>
+  </si>
+  <si>
+    <t>ACAENR80</t>
+  </si>
+  <si>
+    <t>PACA80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no </t>
+  </si>
+  <si>
+    <t>BAPT80</t>
+  </si>
+  <si>
+    <t>TOTMAR80</t>
+  </si>
+  <si>
+    <t>CMAR80</t>
+  </si>
+  <si>
+    <t>MMAR80</t>
+  </si>
+  <si>
+    <t>ACAENR90</t>
+  </si>
+  <si>
+    <t>ELEM90</t>
+  </si>
+  <si>
+    <t>TELEM90</t>
+  </si>
+  <si>
+    <t>LAYSEC90</t>
+  </si>
+  <si>
+    <t>LAYEL90</t>
+  </si>
+  <si>
+    <t>SSA90</t>
+  </si>
+  <si>
+    <t>SEC90</t>
+  </si>
+  <si>
+    <t>TSEC90</t>
+  </si>
+  <si>
+    <t>ACASCH90</t>
+  </si>
+  <si>
+    <t>PACA90</t>
+  </si>
+  <si>
+    <t>BAPT90</t>
+  </si>
+  <si>
+    <t>TOTMAR90</t>
+  </si>
+  <si>
+    <t>CMAR90</t>
+  </si>
+  <si>
+    <t>MMAR90</t>
+  </si>
+  <si>
+    <t>TELEM70</t>
+  </si>
+  <si>
+    <t>ELEM70</t>
+  </si>
+  <si>
+    <t>LAYEL70</t>
+  </si>
+  <si>
+    <t>ACASCH70</t>
+  </si>
+  <si>
+    <t>LEGEND:</t>
+  </si>
+  <si>
+    <t>green = keep variables for regression / clustering</t>
+  </si>
+  <si>
+    <t>green w red lettering = variable names are constant throughout databses</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -354,13 +466,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -375,13 +505,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="fill" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17565,6 +17703,1095 @@
         <row r="1206">
           <cell r="B1206" t="str">
             <v>I-REGION: Region (for use with online analysis) (I-REGION)</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="SCRIP90_data1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="187">
+          <cell r="B187" t="str">
+            <v>Number of secondary students with unspecified grade, 1990 (SUNGRADE)</v>
+          </cell>
+        </row>
+        <row r="188">
+          <cell r="B188" t="str">
+            <v>Number of 12th-grade students, 1990 (TWELVE)</v>
+          </cell>
+        </row>
+        <row r="189">
+          <cell r="B189" t="str">
+            <v>Number of 11th-grade students, 1990 (ELEVEN)</v>
+          </cell>
+        </row>
+        <row r="190">
+          <cell r="B190" t="str">
+            <v>Number of 10th-grade students, 1990 (TENTH)</v>
+          </cell>
+        </row>
+        <row r="191">
+          <cell r="B191" t="str">
+            <v>Number of nineth-grade students, 1990 (NINTH)</v>
+          </cell>
+        </row>
+        <row r="192">
+          <cell r="B192" t="str">
+            <v>Number of eighth-grade students, 1990 (EIGHTH)</v>
+          </cell>
+        </row>
+        <row r="193">
+          <cell r="B193" t="str">
+            <v>Number of seventh-grade students, 1990 (SEVENTH)</v>
+          </cell>
+        </row>
+        <row r="194">
+          <cell r="B194" t="str">
+            <v>Number of sixth-grade students, 1990 (SIXTH)</v>
+          </cell>
+        </row>
+        <row r="195">
+          <cell r="B195" t="str">
+            <v>Number of fifth-grade students, 1990 (FIFTH)</v>
+          </cell>
+        </row>
+        <row r="196">
+          <cell r="B196" t="str">
+            <v>Number of fourth-grade students, 1990 (FOURTH)</v>
+          </cell>
+        </row>
+        <row r="197">
+          <cell r="B197" t="str">
+            <v>Number of third-grade students, 1990 (THIRD)</v>
+          </cell>
+        </row>
+        <row r="198">
+          <cell r="B198" t="str">
+            <v>Number of second-grade students, 1990 (SECOND)</v>
+          </cell>
+        </row>
+        <row r="199">
+          <cell r="B199" t="str">
+            <v>Number of first-grade students, 1990 (FIRST)</v>
+          </cell>
+        </row>
+        <row r="200">
+          <cell r="B200" t="str">
+            <v>Number of kindergarten students, 1990 (KIND)</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="B201" t="str">
+            <v>Number of prekindergarten students, 1990 (PREK)</v>
+          </cell>
+        </row>
+        <row r="202">
+          <cell r="B202" t="str">
+            <v>Number of elementary ungraded students, 1990 (UNGRADE)</v>
+          </cell>
+        </row>
+        <row r="203">
+          <cell r="B203" t="str">
+            <v>Number of secondary non-Catholic students, 1990 (SECNONT)</v>
+          </cell>
+        </row>
+        <row r="204">
+          <cell r="B204" t="str">
+            <v>Number of secondary Catholic students, 1990 (SECCATT)</v>
+          </cell>
+        </row>
+        <row r="205">
+          <cell r="B205" t="str">
+            <v>Number of secondary other students, 1990 (SECOTHRT)</v>
+          </cell>
+        </row>
+        <row r="206">
+          <cell r="B206" t="str">
+            <v>Number of secondary American Indian students, 1990 (SECAIT)</v>
+          </cell>
+        </row>
+        <row r="207">
+          <cell r="B207" t="str">
+            <v>Number of secondary Asian students, 1990 (SECAST)</v>
+          </cell>
+        </row>
+        <row r="208">
+          <cell r="B208" t="str">
+            <v>Number of secondary Hispanic students, 1990 (SECHIST)</v>
+          </cell>
+        </row>
+        <row r="209">
+          <cell r="B209" t="str">
+            <v>Number of secondary black students, 1990 (SECBLT)</v>
+          </cell>
+        </row>
+        <row r="210">
+          <cell r="B210" t="str">
+            <v>Number of elementary non-Catholic students, 1990 (ELNONT)</v>
+          </cell>
+        </row>
+        <row r="211">
+          <cell r="B211" t="str">
+            <v>Number of elementary Catholic students, 1990 (ELCATHT)</v>
+          </cell>
+        </row>
+        <row r="212">
+          <cell r="B212" t="str">
+            <v>Number of elementary other students, 1990 (ELOTHRT)</v>
+          </cell>
+        </row>
+        <row r="213">
+          <cell r="B213" t="str">
+            <v>Number of elementary American Indian students, 1990 (ELAIT)</v>
+          </cell>
+        </row>
+        <row r="214">
+          <cell r="B214" t="str">
+            <v>Number of elementary Asian students, 1990 (ELAST)</v>
+          </cell>
+        </row>
+        <row r="215">
+          <cell r="B215" t="str">
+            <v>Number of elementary Hispanic students, 1990 (ELHIST)</v>
+          </cell>
+        </row>
+        <row r="216">
+          <cell r="B216" t="str">
+            <v>Number of elementary black students, 1990 (ELBLT)</v>
+          </cell>
+        </row>
+        <row r="217">
+          <cell r="B217" t="str">
+            <v>Number of elementary schools in 1990-1991 (see summary documentation for more information) (ELEM90)</v>
+          </cell>
+        </row>
+        <row r="218">
+          <cell r="B218" t="str">
+            <v>Number of secondary schools in 1990-1991 (see summary documentation for more information) (SEC90)</v>
+          </cell>
+        </row>
+        <row r="219">
+          <cell r="B219" t="str">
+            <v>Number of sisters in elementary schools in 1990-1991 (SISEL90)</v>
+          </cell>
+        </row>
+        <row r="220">
+          <cell r="B220" t="str">
+            <v>Number of sisters in secondary schools in 1990-1991 (SISSEC90)</v>
+          </cell>
+        </row>
+        <row r="221">
+          <cell r="B221" t="str">
+            <v>Number of lay teachers in elementary schools in 1990-1991 (LAYEL90)</v>
+          </cell>
+        </row>
+        <row r="222">
+          <cell r="B222" t="str">
+            <v>Number of lay teachers in secondary schools in 1990-1991 (LAYSEC90)</v>
+          </cell>
+        </row>
+        <row r="223">
+          <cell r="B223" t="str">
+            <v>Number of male religious/priests in elementary and secondary schools, combined in 1990-1991 (RELML90)</v>
+          </cell>
+        </row>
+        <row r="224">
+          <cell r="B224" t="str">
+            <v>Total elementary school enrollment in 1990-1991 (TELEM90)</v>
+          </cell>
+        </row>
+        <row r="225">
+          <cell r="B225" t="str">
+            <v>Total secondary school enrollment in 1990-1991 (TSEC90)</v>
+          </cell>
+        </row>
+        <row r="226">
+          <cell r="B226" t="str">
+            <v>Year under consideration, 1990 (YEAR)</v>
+          </cell>
+        </row>
+        <row r="227">
+          <cell r="B227" t="str">
+            <v>Square miles, 1990 (SQMILE90)</v>
+          </cell>
+        </row>
+        <row r="228">
+          <cell r="B228" t="str">
+            <v>Year in which most recent parent diocese started, 1990 (see summary documentation for more information) (PYS90)</v>
+          </cell>
+        </row>
+        <row r="229">
+          <cell r="B229" t="str">
+            <v>Diocese code for PYS90 (see summary documentation for category labels), 1990 (PID90)</v>
+          </cell>
+        </row>
+        <row r="230">
+          <cell r="B230" t="str">
+            <v>Year in which given diocese was first established, 1990 (YRST90)</v>
+          </cell>
+        </row>
+        <row r="231">
+          <cell r="B231" t="str">
+            <v>Number of miscellaneous academies (includes academies for which it was impossible to determine whether elementary or secondary), 1990 (see summary documentation for more information) (ACASCH90)</v>
+          </cell>
+        </row>
+        <row r="232">
+          <cell r="B232" t="str">
+            <v>Miscellaneous academy enrollment, 1990 (ACAENR90)</v>
+          </cell>
+        </row>
+        <row r="233">
+          <cell r="B233" t="str">
+            <v>Percent of miscellaneous academies reporting enrollment, 1990 (PACA90)</v>
+          </cell>
+        </row>
+        <row r="234">
+          <cell r="B234" t="str">
+            <v>Total number of religious teachers, 1990 (ARELT90)</v>
+          </cell>
+        </row>
+        <row r="235">
+          <cell r="B235" t="str">
+            <v>Total number of lay teachers, 1990 (ALAYT90)</v>
+          </cell>
+        </row>
+        <row r="236">
+          <cell r="B236" t="str">
+            <v>Total number of teachers, 1990 (ATTCH90)</v>
+          </cell>
+        </row>
+        <row r="237">
+          <cell r="B237" t="str">
+            <v>Number of miscellaneous academies reporting teachers, 1990 (AREPT90)</v>
+          </cell>
+        </row>
+        <row r="238">
+          <cell r="B238" t="str">
+            <v>Number of single-sex miscellaneous academies, 1990 (SSA90)</v>
+          </cell>
+        </row>
+        <row r="239">
+          <cell r="B239" t="str">
+            <v>Number of orphan asylums, 1990 (see summary documentation for more information) (ORASY90)</v>
+          </cell>
+        </row>
+        <row r="240">
+          <cell r="B240" t="str">
+            <v>Number of orphan inmates, 1990 (ORINM90)</v>
+          </cell>
+        </row>
+        <row r="241">
+          <cell r="B241" t="str">
+            <v>Number of infant asylums, 1990 (INFASY90)</v>
+          </cell>
+        </row>
+        <row r="242">
+          <cell r="B242" t="str">
+            <v>Number of infant inmates, 1990 (INFINM90)</v>
+          </cell>
+        </row>
+        <row r="243">
+          <cell r="B243" t="str">
+            <v>Number of nurseries, 1990 (NURSRY90)</v>
+          </cell>
+        </row>
+        <row r="244">
+          <cell r="B244" t="str">
+            <v>Number of nursery inmates, 1990 (NURINM90)</v>
+          </cell>
+        </row>
+        <row r="245">
+          <cell r="B245" t="str">
+            <v>Number of homes (includes all homes, shelters and protectorories; settlement houses are not included), 1990 (HOMES90)</v>
+          </cell>
+        </row>
+        <row r="246">
+          <cell r="B246" t="str">
+            <v>Total number of children under Catholic care, 1990 (see summary documentation for more information) (CARE90)</v>
+          </cell>
+        </row>
+        <row r="247">
+          <cell r="B247" t="str">
+            <v>Total number of Catholic hospitals, 1990 (HOSP90)</v>
+          </cell>
+        </row>
+        <row r="248">
+          <cell r="B248" t="str">
+            <v>Total number of churches with priests, 1990 (see summary documentation for more information) (CHPRTS90)</v>
+          </cell>
+        </row>
+        <row r="249">
+          <cell r="B249" t="str">
+            <v>Total number of diocesan priests, 1990 (see summary documentation for more information) (DIOPRT90)</v>
+          </cell>
+        </row>
+        <row r="250">
+          <cell r="B250" t="str">
+            <v>Total number of priests, 1990 (TOTPRT90)</v>
+          </cell>
+        </row>
+        <row r="251">
+          <cell r="B251" t="str">
+            <v>Total number of Catholic churches, 1990 (see summary documentation for more information) (TOTCH90)</v>
+          </cell>
+        </row>
+        <row r="252">
+          <cell r="B252" t="str">
+            <v>Total baptisms, 1990 (BAPT90)</v>
+          </cell>
+        </row>
+        <row r="253">
+          <cell r="B253" t="str">
+            <v>Total marriages, 1990 (TOTMAR90)</v>
+          </cell>
+        </row>
+        <row r="254">
+          <cell r="B254" t="str">
+            <v>Catholic marriages, 1990 (CMAR90)</v>
+          </cell>
+        </row>
+        <row r="255">
+          <cell r="B255" t="str">
+            <v>Interfaith marriages, 1990 (MMAR90)</v>
+          </cell>
+        </row>
+        <row r="256">
+          <cell r="B256" t="str">
+            <v>Total Catholic population, 1990 (CATPOP90)</v>
+          </cell>
+        </row>
+        <row r="257">
+          <cell r="B257" t="str">
+            <v>Bishops' date of birth (month/full year), 1990 (DOB90)</v>
+          </cell>
+        </row>
+        <row r="258">
+          <cell r="B258" t="str">
+            <v>Bishops' place of birth, 1990 (POB90)</v>
+          </cell>
+        </row>
+        <row r="259">
+          <cell r="B259" t="str">
+            <v>Bishops' date of consecration (month/full year of when bishop actually took ofice or was consecrated as bishop of the particular diocese), 1990 (DOC90)</v>
+          </cell>
+        </row>
+        <row r="260">
+          <cell r="B260" t="str">
+            <v>Bishops' date ended (month/year of death, retirment, or transferral; coded missing for current bishops), 1990 (DOE90)</v>
+          </cell>
+        </row>
+        <row r="261">
+          <cell r="B261" t="str">
+            <v>Incumbent bishop, 1990 (INC90)</v>
+          </cell>
+        </row>
+        <row r="262">
+          <cell r="B262" t="str">
+            <v>Total number of national parishes (number of parishes listed with a distinct ethnicity), 1990 (NATPAR90)</v>
+          </cell>
+        </row>
+        <row r="263">
+          <cell r="B263" t="str">
+            <v>Ethnicity of national parish 1 (code for most common ethnicity of parish in the diocese, see summary documentation for category labels), 1990 (ETHNP190)</v>
+          </cell>
+        </row>
+        <row r="264">
+          <cell r="B264" t="str">
+            <v>Number of national parishes for ETHNP190, 1990 (NONP190)</v>
+          </cell>
+        </row>
+        <row r="265">
+          <cell r="B265" t="str">
+            <v>Ethnicity of national parish 2 (code for second-most-common ethnicity of parish in the diocese, see summary documentation for category labels), 1990 (ETHNP290)</v>
+          </cell>
+        </row>
+        <row r="266">
+          <cell r="B266" t="str">
+            <v>Number of national parishes for ETHNP960, 1990 (NONP290)</v>
+          </cell>
+        </row>
+        <row r="267">
+          <cell r="B267" t="str">
+            <v>Ethnicity of national parish 3 (code for third-most-common ethnicity in the diocese, see summary documentation for category labels), 1990 (ETHNP390)</v>
+          </cell>
+        </row>
+        <row r="268">
+          <cell r="B268" t="str">
+            <v>Number of national parishes for ETHNP390, 1990 (NONP390)</v>
+          </cell>
+        </row>
+        <row r="269">
+          <cell r="B269" t="str">
+            <v>Number of national parishes with schools, 1990 (NPSCH90)</v>
+          </cell>
+        </row>
+        <row r="270">
+          <cell r="B270" t="str">
+            <v>Total number of regular parishes, 1990 (REGPAR90)</v>
+          </cell>
+        </row>
+        <row r="271">
+          <cell r="B271" t="str">
+            <v>Number of regular parishes with schools, 1990 (RPSCH90)</v>
+          </cell>
+        </row>
+        <row r="272">
+          <cell r="B272" t="str">
+            <v>Number of ethnic missions in regular parishes, 1990 (EMRP90)</v>
+          </cell>
+        </row>
+        <row r="273">
+          <cell r="B273" t="str">
+            <v>Number of ethnicities of national parishes, 1990 (NOETHP90)</v>
+          </cell>
+        </row>
+        <row r="274">
+          <cell r="B274" t="str">
+            <v>Number of ethnicities of ethnic missions, 1990 (NOETHM90)</v>
+          </cell>
+        </row>
+        <row r="275">
+          <cell r="B275" t="str">
+            <v>Mainline Protestant churches-number of churches, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SMANCH90)</v>
+          </cell>
+        </row>
+        <row r="276">
+          <cell r="B276" t="str">
+            <v>Mainline Protestant churches-number of members, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SMANCM90)</v>
+          </cell>
+        </row>
+        <row r="277">
+          <cell r="B277" t="str">
+            <v>Mainline Protestant churches-number of adherents, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SMANAD90)</v>
+          </cell>
+        </row>
+        <row r="278">
+          <cell r="B278" t="str">
+            <v>Other Protestant churches-number of churches, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SOTHCH90)</v>
+          </cell>
+        </row>
+        <row r="279">
+          <cell r="B279" t="str">
+            <v>Other Protestant churches-number of members, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SOTHCM90)</v>
+          </cell>
+        </row>
+        <row r="280">
+          <cell r="B280" t="str">
+            <v>Other Protestant churches-number of adherents, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SOTHAD90)</v>
+          </cell>
+        </row>
+        <row r="281">
+          <cell r="B281" t="str">
+            <v>Catholic churches-number of churches, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SCATCH90)</v>
+          </cell>
+        </row>
+        <row r="282">
+          <cell r="B282" t="str">
+            <v>Catholic churches-number of members, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SCATCM90)</v>
+          </cell>
+        </row>
+        <row r="283">
+          <cell r="B283" t="str">
+            <v>Catholic churches-number of adherents, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SCATAD90)</v>
+          </cell>
+        </row>
+        <row r="284">
+          <cell r="B284" t="str">
+            <v>Jewish synagogues (estimated)-number of synagogues, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SJEWCH90)</v>
+          </cell>
+        </row>
+        <row r="285">
+          <cell r="B285" t="str">
+            <v>Jewish synagogues (estimated)-number of members, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SJEWCM90)</v>
+          </cell>
+        </row>
+        <row r="286">
+          <cell r="B286" t="str">
+            <v>Jewish synagogues (estimated)-number of adherents, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SJEWAD90)</v>
+          </cell>
+        </row>
+        <row r="287">
+          <cell r="B287" t="str">
+            <v>Total population, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SGTPOP90)</v>
+          </cell>
+        </row>
+        <row r="288">
+          <cell r="B288" t="str">
+            <v>Total number of churches, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SCHRCH90)</v>
+          </cell>
+        </row>
+        <row r="289">
+          <cell r="B289" t="str">
+            <v>Total number of members, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SMBRS90)</v>
+          </cell>
+        </row>
+        <row r="290">
+          <cell r="B290" t="str">
+            <v>Total number of adherents, 1990 (determined by sum of data collected from counties reporting information in each diocese) (SADHER90)</v>
+          </cell>
+        </row>
+        <row r="291">
+          <cell r="B291" t="str">
+            <v>Total population, 1990 (TPOP90)</v>
+          </cell>
+        </row>
+        <row r="292">
+          <cell r="B292" t="str">
+            <v>Total number of families, 1990 (FAM90)</v>
+          </cell>
+        </row>
+        <row r="293">
+          <cell r="B293" t="str">
+            <v>Urban population, 1990 (URBAN190)</v>
+          </cell>
+        </row>
+        <row r="294">
+          <cell r="B294" t="str">
+            <v>Suburban population, 1990 (URBAN290)</v>
+          </cell>
+        </row>
+        <row r="295">
+          <cell r="B295" t="str">
+            <v>White population, 1990 (WHITE90)</v>
+          </cell>
+        </row>
+        <row r="296">
+          <cell r="B296" t="str">
+            <v>Black population, 1990 (BLACK90)</v>
+          </cell>
+        </row>
+        <row r="297">
+          <cell r="B297" t="str">
+            <v>Native American population, 1990 (NATIVE90)</v>
+          </cell>
+        </row>
+        <row r="298">
+          <cell r="B298" t="str">
+            <v>Asian-Pacific population, 1990 (ASIAN90)</v>
+          </cell>
+        </row>
+        <row r="299">
+          <cell r="B299" t="str">
+            <v>Hispanic population, 1990 (HISP90)</v>
+          </cell>
+        </row>
+        <row r="300">
+          <cell r="B300" t="str">
+            <v>Number of married-couple families with own children under 18, 1990 (MAR190)</v>
+          </cell>
+        </row>
+        <row r="301">
+          <cell r="B301" t="str">
+            <v>Number of married-couple families with no own children under 18, 1990 (MAR290)</v>
+          </cell>
+        </row>
+        <row r="302">
+          <cell r="B302" t="str">
+            <v>Number of female householders (no husband present) with own children under 18, 1990 (FHF190)</v>
+          </cell>
+        </row>
+        <row r="303">
+          <cell r="B303" t="str">
+            <v>Number of female householders (no husband present) with no own children under 18, 1990 (FHF290)</v>
+          </cell>
+        </row>
+        <row r="304">
+          <cell r="B304" t="str">
+            <v>Number of employed male civilians 16 years and older,1990 (MCE90)</v>
+          </cell>
+        </row>
+        <row r="305">
+          <cell r="B305" t="str">
+            <v>Number of employed female civilians 16 years and older, 1990 (MCU90)</v>
+          </cell>
+        </row>
+        <row r="306">
+          <cell r="B306" t="str">
+            <v>Number of unemployed male civilians 16 years and older, 1990 (FCE90)</v>
+          </cell>
+        </row>
+        <row r="307">
+          <cell r="B307" t="str">
+            <v>Number of unemployed female civilians 16 years and older, 1990 (FCU90)</v>
+          </cell>
+        </row>
+        <row r="308">
+          <cell r="B308" t="str">
+            <v>Number of households with an income less than $5,000, 1989 (INC189)</v>
+          </cell>
+        </row>
+        <row r="309">
+          <cell r="B309" t="str">
+            <v>Number of households with an income between $5,000 and $9,999, 1989 (INC289)</v>
+          </cell>
+        </row>
+        <row r="310">
+          <cell r="B310" t="str">
+            <v>Number of households with an income between $10,000 and $12,499, 1989 (INC389)</v>
+          </cell>
+        </row>
+        <row r="311">
+          <cell r="B311" t="str">
+            <v>Number of households with an income between $12,500 and $14,999, 1989 (INC489)</v>
+          </cell>
+        </row>
+        <row r="312">
+          <cell r="B312" t="str">
+            <v>Number of households with an income between $15,000 and $17,499, 1989 (INC589)</v>
+          </cell>
+        </row>
+        <row r="313">
+          <cell r="B313" t="str">
+            <v>Number of households with an income between $17,500 and $19,999, 1989 (INC689)</v>
+          </cell>
+        </row>
+        <row r="314">
+          <cell r="B314" t="str">
+            <v>Number of households with an income between $20,000 and $22,499, 1989 (INC789)</v>
+          </cell>
+        </row>
+        <row r="315">
+          <cell r="B315" t="str">
+            <v>Number of households with an income between $22,500 and $24,999, 1989 (INC889)</v>
+          </cell>
+        </row>
+        <row r="316">
+          <cell r="B316" t="str">
+            <v>Number of households with an income between $25,000 and $27,499, 1989 (INC989)</v>
+          </cell>
+        </row>
+        <row r="317">
+          <cell r="B317" t="str">
+            <v>Number of households with an income between $27,500 and $29,999, 1989 (INC1089)</v>
+          </cell>
+        </row>
+        <row r="318">
+          <cell r="B318" t="str">
+            <v>Number of households with an income between $30,000 and $32,499, 1989 (INC1189)</v>
+          </cell>
+        </row>
+        <row r="319">
+          <cell r="B319" t="str">
+            <v>Number of households with an income between $32,500 and $34,999, 1989 (INC1289)</v>
+          </cell>
+        </row>
+        <row r="320">
+          <cell r="B320" t="str">
+            <v>Number of households with an income between $35,000 and $37,499, 1989 (INC1389)</v>
+          </cell>
+        </row>
+        <row r="321">
+          <cell r="B321" t="str">
+            <v>Number of households with an income between $37,500 and $39,999, 1989 (INC1489)</v>
+          </cell>
+        </row>
+        <row r="322">
+          <cell r="B322" t="str">
+            <v>Number of households with an income between $40,000 and $42,499, 1989 (INC1589)</v>
+          </cell>
+        </row>
+        <row r="323">
+          <cell r="B323" t="str">
+            <v>Number of households with an income between $42,500 and $44,999, 1989 (INC1689)</v>
+          </cell>
+        </row>
+        <row r="324">
+          <cell r="B324" t="str">
+            <v>Number of households with an income between $45,000 and $47,499, 1989 (INC1789)</v>
+          </cell>
+        </row>
+        <row r="325">
+          <cell r="B325" t="str">
+            <v>Number of households with an income between $47,500 and $49,999, 1989 (INC1889)</v>
+          </cell>
+        </row>
+        <row r="326">
+          <cell r="B326" t="str">
+            <v>Number of households with an income between $50,000 and $54,999, 1989 (INC1989)</v>
+          </cell>
+        </row>
+        <row r="327">
+          <cell r="B327" t="str">
+            <v>Number of households with an income between $55,000 and $59,999, 1989 (INC2089)</v>
+          </cell>
+        </row>
+        <row r="328">
+          <cell r="B328" t="str">
+            <v>Number of households with an income between $60,000 and $74,999, 1989 (INC2189)</v>
+          </cell>
+        </row>
+        <row r="329">
+          <cell r="B329" t="str">
+            <v>Number of households with an income between $75,000 and $99,999, 1989 (INC2289)</v>
+          </cell>
+        </row>
+        <row r="330">
+          <cell r="B330" t="str">
+            <v>Number of households with an income between $100,000 and $124,999, 1989 (INC2389)</v>
+          </cell>
+        </row>
+        <row r="331">
+          <cell r="B331" t="str">
+            <v>Number of households with an income between $125,000 and $149,999, 1989 (INC2489)</v>
+          </cell>
+        </row>
+        <row r="332">
+          <cell r="B332" t="str">
+            <v>Number of households with an income over $150,000, 1989 (INC2589)</v>
+          </cell>
+        </row>
+        <row r="333">
+          <cell r="B333" t="str">
+            <v>Mean of median household income, 1989 (MHINC89)</v>
+          </cell>
+        </row>
+        <row r="334">
+          <cell r="B334" t="str">
+            <v>Mean of median family income, 1989 (MFINC89)</v>
+          </cell>
+        </row>
+        <row r="335">
+          <cell r="B335" t="str">
+            <v>Mean of per capita income, 1989 (PCINC89)</v>
+          </cell>
+        </row>
+        <row r="336">
+          <cell r="B336" t="str">
+            <v>Number of persons under 5 years of age below poverty level, 1989 (PPTY189)</v>
+          </cell>
+        </row>
+        <row r="337">
+          <cell r="B337" t="str">
+            <v>Number of 5-year-olds below poverty level, 1989 (PPTY289)</v>
+          </cell>
+        </row>
+        <row r="338">
+          <cell r="B338" t="str">
+            <v>Number of persons 6 to 11 years old below poverty level, 1989 (PPTY389)</v>
+          </cell>
+        </row>
+        <row r="339">
+          <cell r="B339" t="str">
+            <v>Number of persons 12 to 17 years old below poverty level, 1989 (PPTY489)</v>
+          </cell>
+        </row>
+        <row r="340">
+          <cell r="B340" t="str">
+            <v>Number of persons 18 to 24 years old below poverty level, 1989 (PPTY589)</v>
+          </cell>
+        </row>
+        <row r="341">
+          <cell r="B341" t="str">
+            <v>Number of persons 25 to 34 years old below poverty level, 1989 (PPTY689)</v>
+          </cell>
+        </row>
+        <row r="342">
+          <cell r="B342" t="str">
+            <v>Number of persons 35 to 44 years old below poverty level, 1989 (PPTY789)</v>
+          </cell>
+        </row>
+        <row r="343">
+          <cell r="B343" t="str">
+            <v>Number of persons 45 to 54 years old below poverty level, 1989 (PPTY889)</v>
+          </cell>
+        </row>
+        <row r="344">
+          <cell r="B344" t="str">
+            <v>Number of persons 55 to 59 years old below poverty level, 1989 (PPTY989)</v>
+          </cell>
+        </row>
+        <row r="345">
+          <cell r="B345" t="str">
+            <v>Number of persons 60 to 64 years old below poverty level, 1989 (PPTY1089)</v>
+          </cell>
+        </row>
+        <row r="346">
+          <cell r="B346" t="str">
+            <v>Number of persons 65 to 74 years old below poverty level, 1989 (PPTY1189)</v>
+          </cell>
+        </row>
+        <row r="347">
+          <cell r="B347" t="str">
+            <v>Number of persons 75 years and older below poverty level, 1989 (PPTY1289)</v>
+          </cell>
+        </row>
+        <row r="348">
+          <cell r="B348" t="str">
+            <v>Number of married-couple families below poverty level with related children under 5 years, 1989 (FPTY189)</v>
+          </cell>
+        </row>
+        <row r="349">
+          <cell r="B349" t="str">
+            <v>Number of married-couples below poverty level with related children 5 to 17 years old, 1989 (FPTY289)</v>
+          </cell>
+        </row>
+        <row r="350">
+          <cell r="B350" t="str">
+            <v>Number of married-couples below poverty level with related children under 5 years and 5 to 17 years old, 1989 (FPTY389)</v>
+          </cell>
+        </row>
+        <row r="351">
+          <cell r="B351" t="str">
+            <v>Number of married-couples below poverty level with no related children under 18 years, 1989 (FPTY489)</v>
+          </cell>
+        </row>
+        <row r="352">
+          <cell r="B352" t="str">
+            <v>Number of male householders (no wife present) below the poverty level with related children under 5 years, 1989 (FPTY589)</v>
+          </cell>
+        </row>
+        <row r="353">
+          <cell r="B353" t="str">
+            <v>Number of male householders (no wife present) below the poverty level with related children 5 to 17 years old, 1989 (FPTY689)</v>
+          </cell>
+        </row>
+        <row r="354">
+          <cell r="B354" t="str">
+            <v>Number of male householders (no wife present) below the poverty level with related children under 5 years and 5 to 17 years old, 1989 (FPTY789)</v>
+          </cell>
+        </row>
+        <row r="355">
+          <cell r="B355" t="str">
+            <v>Number of male householders (no wife present) below the poverty level with no own children under 18. 1989 (FPTY889)</v>
+          </cell>
+        </row>
+        <row r="356">
+          <cell r="B356" t="str">
+            <v>Number of female householders (no husband present) below poverty level with children under 5 years, 1989 (FPTY989)</v>
+          </cell>
+        </row>
+        <row r="357">
+          <cell r="B357" t="str">
+            <v>Number of female householders (no husband present) below poverty level with related children 5 to 17 years old, 1989 (FPTY1089)</v>
+          </cell>
+        </row>
+        <row r="358">
+          <cell r="B358" t="str">
+            <v>Number of female householders (no husband present) below poverty level with related children under 5 years and 5 to17 years old, 1989 (FPTY1189)</v>
+          </cell>
+        </row>
+        <row r="359">
+          <cell r="B359" t="str">
+            <v>Number of female householders (no husband present) below poverty level with no related children under 18 years, 1989 (FPTY1289)</v>
+          </cell>
+        </row>
+        <row r="360">
+          <cell r="B360" t="str">
+            <v>Number of married-couple families, 1990 (MAR90)</v>
+          </cell>
+        </row>
+        <row r="361">
+          <cell r="B361" t="str">
+            <v>Number of female householders, 1990 (FHF90)</v>
+          </cell>
+        </row>
+        <row r="362">
+          <cell r="B362" t="str">
+            <v>Total urban populations, 1990 (URBAN90)</v>
+          </cell>
+        </row>
+        <row r="363">
+          <cell r="B363" t="str">
+            <v>Number of employed civilians, 1990 (CIVEMP90)</v>
+          </cell>
+        </row>
+        <row r="364">
+          <cell r="B364" t="str">
+            <v>Number of unemployed civilians, 1990 (CIVUNP90)</v>
+          </cell>
+        </row>
+        <row r="365">
+          <cell r="B365" t="str">
+            <v>Number of persons below poverty level, 1989 (PERPOV89)</v>
+          </cell>
+        </row>
+        <row r="366">
+          <cell r="B366" t="str">
+            <v>Number of families below poverty level, 1989 (FAMPOV89)</v>
+          </cell>
+        </row>
+        <row r="367">
+          <cell r="B367" t="str">
+            <v>Male population, 1990 (MALES90)</v>
+          </cell>
+        </row>
+        <row r="368">
+          <cell r="B368" t="str">
+            <v>Female population, 1990 (FEMALE90)</v>
+          </cell>
+        </row>
+        <row r="369">
+          <cell r="B369" t="str">
+            <v>Population of other races, 1990 (OTHRAC90)</v>
+          </cell>
+        </row>
+        <row r="370">
+          <cell r="B370" t="str">
+            <v>Number of children less than 1 year, 1990 (ALT190)</v>
+          </cell>
+        </row>
+        <row r="371">
+          <cell r="B371" t="str">
+            <v>Number of 1- and 2-year-olds, 1990 (A1_290)</v>
+          </cell>
+        </row>
+        <row r="372">
+          <cell r="B372" t="str">
+            <v>Number of 3- and 4-year-olds, 1990 (A3_490)</v>
+          </cell>
+        </row>
+        <row r="373">
+          <cell r="B373" t="str">
+            <v>Number of 5- year-olds, 1990 (A590)</v>
+          </cell>
+        </row>
+        <row r="374">
+          <cell r="B374" t="str">
+            <v>Number of 6- year-olds, 1990 (A690)</v>
+          </cell>
+        </row>
+        <row r="375">
+          <cell r="B375" t="str">
+            <v>Number of 7- to 9-year-olds, 1990 (A7_990)</v>
+          </cell>
+        </row>
+        <row r="376">
+          <cell r="B376" t="str">
+            <v>Number of 10- and 11-year-olds, 1990 (A10_1190)</v>
+          </cell>
+        </row>
+        <row r="377">
+          <cell r="B377" t="str">
+            <v>Number of 12- and 13-year-olds, 1990 (A12_1390)</v>
+          </cell>
+        </row>
+        <row r="378">
+          <cell r="B378" t="str">
+            <v>Number of 14-year-olds, 1990 (A1490)</v>
+          </cell>
+        </row>
+        <row r="379">
+          <cell r="B379" t="str">
+            <v>Number of 15-year-olds, 1990 (A1590)</v>
+          </cell>
+        </row>
+        <row r="380">
+          <cell r="B380" t="str">
+            <v>Number of 16-year-olds, 1990 (A1690)</v>
+          </cell>
+        </row>
+        <row r="381">
+          <cell r="B381" t="str">
+            <v>Number of 17-year-olds, 1990 (A1790)</v>
+          </cell>
+        </row>
+        <row r="382">
+          <cell r="B382" t="str">
+            <v>Number of 18-year-olds, 1990 (A1890)</v>
+          </cell>
+        </row>
+        <row r="383">
+          <cell r="B383" t="str">
+            <v>Number of 19-year-olds, 1990 (A1990)</v>
+          </cell>
+        </row>
+        <row r="384">
+          <cell r="B384" t="str">
+            <v>Number of 20-year-olds, 1990 (A2090)</v>
+          </cell>
+        </row>
+        <row r="385">
+          <cell r="B385" t="str">
+            <v>Number of 21-year-olds, 1990 (A2190)</v>
+          </cell>
+        </row>
+        <row r="386">
+          <cell r="B386" t="str">
+            <v>Number of 22- to 24-year-olds, 1990 (A22_2490)</v>
+          </cell>
+        </row>
+        <row r="387">
+          <cell r="B387" t="str">
+            <v>Number of 25- to 29-year-olds, 1990 (A25_2990)</v>
+          </cell>
+        </row>
+        <row r="388">
+          <cell r="B388" t="str">
+            <v>Number of 30- to 34-year-olds, 1990 (A30_3490)</v>
+          </cell>
+        </row>
+        <row r="389">
+          <cell r="B389" t="str">
+            <v>Number of 35- to 39-year-olds, 1990 (A35_3990)</v>
+          </cell>
+        </row>
+        <row r="390">
+          <cell r="B390" t="str">
+            <v>Number of 40- to 44-year-olds, 1990 (A40_4490)</v>
+          </cell>
+        </row>
+        <row r="391">
+          <cell r="B391" t="str">
+            <v>Number of 45- to 49-year-olds, 1990 (A45_4990)</v>
+          </cell>
+        </row>
+        <row r="392">
+          <cell r="B392" t="str">
+            <v>Number of 50- to 54-year-olds, 1990 (A50_5490)</v>
+          </cell>
+        </row>
+        <row r="393">
+          <cell r="B393" t="str">
+            <v>Number of 55- to 59-year-olds, 1990 (A55_5990)</v>
+          </cell>
+        </row>
+        <row r="394">
+          <cell r="B394" t="str">
+            <v>Number of 60- to 61-year-olds, 1990 (A60_6190)</v>
+          </cell>
+        </row>
+        <row r="395">
+          <cell r="B395" t="str">
+            <v>Number of 62- to 64-year-olds, 1990 (A62_6490)</v>
+          </cell>
+        </row>
+        <row r="396">
+          <cell r="B396" t="str">
+            <v>Number of 65 to 69-year-olds, 1990 (A65_6990)</v>
+          </cell>
+        </row>
+        <row r="397">
+          <cell r="B397" t="str">
+            <v>Number of 70- to 74-year-olds, 1990 (A70_7490)</v>
+          </cell>
+        </row>
+        <row r="398">
+          <cell r="B398" t="str">
+            <v>Number of 75- to 79-year-olds, 1990 (A75_7990)</v>
+          </cell>
+        </row>
+        <row r="399">
+          <cell r="B399" t="str">
+            <v>Number of 80- to 84-year-olds, 1990 (A80_8490)</v>
+          </cell>
+        </row>
+        <row r="400">
+          <cell r="B400" t="str">
+            <v>Number of 85-year-olds and older, 1990 (A85UP90)</v>
+          </cell>
+        </row>
+        <row r="401">
+          <cell r="B401" t="str">
+            <v>Region (REGION)</v>
           </cell>
         </row>
       </sheetData>
@@ -17870,10 +19097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21A5F18-BAEF-2145-9C32-DFF5C6077E54}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17882,7 +19109,7 @@
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -17899,639 +19126,889 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20">
-      <c r="A2" s="2">
+    <row r="2" spans="1:11" ht="20">
+      <c r="A2" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1),LEN(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B2">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1),LEN(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1),LEN(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1),LEN(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1),LEN(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1))-1,1,7),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1),LEN(MID(F2,FIND("(",F2)+1,FIND(")",F2)-FIND("(",F2)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="J2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="20">
-      <c r="A3" s="2">
+    <row r="3" spans="1:11" ht="20">
+      <c r="A3" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1),LEN(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B3">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1),LEN(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1),LEN(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="C3">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1),LEN(MID(F3,FIND("(",F3)+1,FIND(")",F3)-FIND("(",F3)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
+      <c r="K3" t="s">
+        <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20">
-      <c r="A4" s="2">
+    <row r="4" spans="1:11" ht="20">
+      <c r="A4" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1),LEN(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B4">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1),LEN(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1),LEN(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="C4">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1),LEN(MID(F4,FIND("(",F4)+1,FIND(")",F4)-FIND("(",F4)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20">
-      <c r="A5" s="2">
+    <row r="5" spans="1:11" ht="20">
+      <c r="A5" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1),LEN(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B5">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1),LEN(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1),LEN(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C5">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1),LEN(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1),LEN(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1))-1,1,7),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1),LEN(MID(F5,FIND("(",F5)+1,FIND(")",F5)-FIND("(",F5)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20">
-      <c r="A6" s="2">
+    <row r="6" spans="1:11" ht="20">
+      <c r="A6" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1),LEN(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B6">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1),LEN(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1),LEN(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="C6">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1),LEN(MID(F6,FIND("(",F6)+1,FIND(")",F6)-FIND("(",F6)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20">
-      <c r="A7" s="2">
+    <row r="7" spans="1:11" ht="20">
+      <c r="A7" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1),LEN(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B7">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1),LEN(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1),LEN(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C7">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1),LEN(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1),LEN(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1))-1,1,7),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1),LEN(MID(F7,FIND("(",F7)+1,FIND(")",F7)-FIND("(",F7)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20">
-      <c r="A8" s="2">
+    <row r="8" spans="1:11" ht="20">
+      <c r="A8" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F8,FIND("(",F8)+1,FIND(")",F8)-FIND("(",F8)-1),LEN(MID(F8,FIND("(",F8)+1,FIND(")",F8)-FIND("(",F8)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B8">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F8,FIND("(",F8)+1,FIND(")",F8)-FIND("(",F8)-1),LEN(MID(F8,FIND("(",F8)+1,FIND(")",F8)-FIND("(",F8)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F8,FIND("(",F8)+1,FIND(")",F8)-FIND("(",F8)-1),LEN(MID(F8,FIND("(",F8)+1,FIND(")",F8)-FIND("(",F8)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20">
-      <c r="A9" s="2">
+    <row r="9" spans="1:11" ht="20">
+      <c r="A9" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F9,FIND("(",F9)+1,FIND(")",F9)-FIND("(",F9)-1),LEN(MID(F9,FIND("(",F9)+1,FIND(")",F9)-FIND("(",F9)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B9">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F9,FIND("(",F9)+1,FIND(")",F9)-FIND("(",F9)-1),LEN(MID(F9,FIND("(",F9)+1,FIND(")",F9)-FIND("(",F9)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F9,FIND("(",F9)+1,FIND(")",F9)-FIND("(",F9)-1),LEN(MID(F9,FIND("(",F9)+1,FIND(")",F9)-FIND("(",F9)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="D9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20">
-      <c r="A10" s="2">
+    <row r="10" spans="1:11" ht="20">
+      <c r="A10" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1),LEN(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B10">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1),LEN(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1),LEN(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1),LEN(MID(F10,FIND("(",F10)+1,FIND(")",F10)-FIND("(",F10)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20">
-      <c r="A11" s="2">
+    <row r="11" spans="1:11" ht="20">
+      <c r="A11" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F11,FIND("(",F11)+1,FIND(")",F11)-FIND("(",F11)-1),LEN(MID(F11,FIND("(",F11)+1,FIND(")",F11)-FIND("(",F11)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B11">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F11,FIND("(",F11)+1,FIND(")",F11)-FIND("(",F11)-1),LEN(MID(F11,FIND("(",F11)+1,FIND(")",F11)-FIND("(",F11)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F11,FIND("(",F11)+1,FIND(")",F11)-FIND("(",F11)-1),LEN(MID(F11,FIND("(",F11)+1,FIND(")",F11)-FIND("(",F11)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20">
-      <c r="A12" s="2">
+    <row r="12" spans="1:11" ht="20">
+      <c r="A12" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1),LEN(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B12">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1),LEN(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1),LEN(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1),LEN(MID(F12,FIND("(",F12)+1,FIND(")",F12)-FIND("(",F12)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20">
-      <c r="A13" s="2">
+    <row r="13" spans="1:11" ht="20">
+      <c r="A13" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F13,FIND("(",F13)+1,FIND(")",F13)-FIND("(",F13)-1),LEN(MID(F13,FIND("(",F13)+1,FIND(")",F13)-FIND("(",F13)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B13">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F13,FIND("(",F13)+1,FIND(")",F13)-FIND("(",F13)-1),LEN(MID(F13,FIND("(",F13)+1,FIND(")",F13)-FIND("(",F13)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F13,FIND("(",F13)+1,FIND(")",F13)-FIND("(",F13)-1),LEN(MID(F13,FIND("(",F13)+1,FIND(")",F13)-FIND("(",F13)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20">
-      <c r="A14" s="2">
+    <row r="14" spans="1:11" ht="20">
+      <c r="A14" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F14,FIND("(",F14)+1,FIND(")",F14)-FIND("(",F14)-1),LEN(MID(F14,FIND("(",F14)+1,FIND(")",F14)-FIND("(",F14)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B14">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F14,FIND("(",F14)+1,FIND(")",F14)-FIND("(",F14)-1),LEN(MID(F14,FIND("(",F14)+1,FIND(")",F14)-FIND("(",F14)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F14,FIND("(",F14)+1,FIND(")",F14)-FIND("(",F14)-1),LEN(MID(F14,FIND("(",F14)+1,FIND(")",F14)-FIND("(",F14)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20">
-      <c r="A15" s="2">
+    <row r="15" spans="1:11" ht="20">
+      <c r="A15" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F15,FIND("(",F15)+1,FIND(")",F15)-FIND("(",F15)-1),LEN(MID(F15,FIND("(",F15)+1,FIND(")",F15)-FIND("(",F15)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B15">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F15,FIND("(",F15)+1,FIND(")",F15)-FIND("(",F15)-1),LEN(MID(F15,FIND("(",F15)+1,FIND(")",F15)-FIND("(",F15)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F15,FIND("(",F15)+1,FIND(")",F15)-FIND("(",F15)-1),LEN(MID(F15,FIND("(",F15)+1,FIND(")",F15)-FIND("(",F15)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="D15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20">
-      <c r="A16" s="2">
+    <row r="16" spans="1:11" ht="20">
+      <c r="A16" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F16,FIND("(",F16)+1,FIND(")",F16)-FIND("(",F16)-1),LEN(MID(F16,FIND("(",F16)+1,FIND(")",F16)-FIND("(",F16)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B16">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F16,FIND("(",F16)+1,FIND(")",F16)-FIND("(",F16)-1),LEN(MID(F16,FIND("(",F16)+1,FIND(")",F16)-FIND("(",F16)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F16,FIND("(",F16)+1,FIND(")",F16)-FIND("(",F16)-1),LEN(MID(F16,FIND("(",F16)+1,FIND(")",F16)-FIND("(",F16)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F17,FIND("(",F17)+1,FIND(")",F17)-FIND("(",F17)-1),LEN(MID(F17,FIND("(",F17)+1,FIND(")",F17)-FIND("(",F17)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B17">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F17,FIND("(",F17)+1,FIND(")",F17)-FIND("(",F17)-1),LEN(MID(F17,FIND("(",F17)+1,FIND(")",F17)-FIND("(",F17)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F17,FIND("(",F17)+1,FIND(")",F17)-FIND("(",F17)-1),LEN(MID(F17,FIND("(",F17)+1,FIND(")",F17)-FIND("(",F17)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="D17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F18,FIND("(",F18)+1,FIND(")",F18)-FIND("(",F18)-1),LEN(MID(F18,FIND("(",F18)+1,FIND(")",F18)-FIND("(",F18)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B18">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F18,FIND("(",F18)+1,FIND(")",F18)-FIND("(",F18)-1),LEN(MID(F18,FIND("(",F18)+1,FIND(")",F18)-FIND("(",F18)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F18,FIND("(",F18)+1,FIND(")",F18)-FIND("(",F18)-1),LEN(MID(F18,FIND("(",F18)+1,FIND(")",F18)-FIND("(",F18)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F19,FIND("(",F19)+1,FIND(")",F19)-FIND("(",F19)-1),LEN(MID(F19,FIND("(",F19)+1,FIND(")",F19)-FIND("(",F19)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B19">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F19,FIND("(",F19)+1,FIND(")",F19)-FIND("(",F19)-1),LEN(MID(F19,FIND("(",F19)+1,FIND(")",F19)-FIND("(",F19)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F19,FIND("(",F19)+1,FIND(")",F19)-FIND("(",F19)-1),LEN(MID(F19,FIND("(",F19)+1,FIND(")",F19)-FIND("(",F19)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F20,FIND("(",F20)+1,FIND(")",F20)-FIND("(",F20)-1),LEN(MID(F20,FIND("(",F20)+1,FIND(")",F20)-FIND("(",F20)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B20">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F20,FIND("(",F20)+1,FIND(")",F20)-FIND("(",F20)-1),LEN(MID(F20,FIND("(",F20)+1,FIND(")",F20)-FIND("(",F20)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F20,FIND("(",F20)+1,FIND(")",F20)-FIND("(",F20)-1),LEN(MID(F20,FIND("(",F20)+1,FIND(")",F20)-FIND("(",F20)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1),LEN(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B21">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1),LEN(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1),LEN(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C21">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1),LEN(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1),LEN(MID(F21,FIND("(",F21)+1,FIND(")",F21)-FIND("(",F21)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1),LEN(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B22">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1),LEN(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1),LEN(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C22">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1),LEN(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1),LEN(MID(F22,FIND("(",F22)+1,FIND(")",F22)-FIND("(",F22)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="20">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1),LEN(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B23">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1),LEN(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1),LEN(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C23">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1),LEN(MID(F23,FIND("(",F23)+1,FIND(")",F23)-FIND("(",F23)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="20">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1),LEN(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B24">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1),LEN(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1),LEN(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C24">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1),LEN(MID(F24,FIND("(",F24)+1,FIND(")",F24)-FIND("(",F24)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1),LEN(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B25">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1),LEN(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1),LEN(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C25">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1),LEN(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1),LEN(MID(F25,FIND("(",F25)+1,FIND(")",F25)-FIND("(",F25)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="20">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1),LEN(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B26">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1),LEN(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1),LEN(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C26">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1),LEN(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1),LEN(MID(F26,FIND("(",F26)+1,FIND(")",F26)-FIND("(",F26)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="20">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1),LEN(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B27">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1),LEN(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1),LEN(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C27">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1),LEN(MID(F27,FIND("(",F27)+1,FIND(")",F27)-FIND("(",F27)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1),LEN(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B28">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1),LEN(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1),LEN(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C28">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1),LEN(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1),LEN(MID(F28,FIND("(",F28)+1,FIND(")",F28)-FIND("(",F28)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="20">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1),LEN(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B29">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1),LEN(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1),LEN(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C29">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1),LEN(MID(F29,FIND("(",F29)+1,FIND(")",F29)-FIND("(",F29)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="20">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1),LEN(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B30">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1),LEN(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1),LEN(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C30">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1),LEN(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1),LEN(MID(F30,FIND("(",F30)+1,FIND(")",F30)-FIND("(",F30)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="20">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1),LEN(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B31">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1),LEN(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1),LEN(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C31">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1),LEN(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1),LEN(MID(F31,FIND("(",F31)+1,FIND(")",F31)-FIND("(",F31)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="20">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1),LEN(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B32">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1),LEN(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1),LEN(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C32">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1),LEN(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1),LEN(MID(F32,FIND("(",F32)+1,FIND(")",F32)-FIND("(",F32)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="20">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1),LEN(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B33">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1),LEN(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1),LEN(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C33">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1),LEN(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1),LEN(MID(F33,FIND("(",F33)+1,FIND(")",F33)-FIND("(",F33)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F34,FIND("(",F34)+1,FIND(")",F34)-FIND("(",F34)-1),LEN(MID(F34,FIND("(",F34)+1,FIND(")",F34)-FIND("(",F34)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B34">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F34,FIND("(",F34)+1,FIND(")",F34)-FIND("(",F34)-1),LEN(MID(F34,FIND("(",F34)+1,FIND(")",F34)-FIND("(",F34)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F34,FIND("(",F34)+1,FIND(")",F34)-FIND("(",F34)-1),LEN(MID(F34,FIND("(",F34)+1,FIND(")",F34)-FIND("(",F34)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1),LEN(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B35">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1),LEN(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1),LEN(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C35">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1),LEN(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1),LEN(MID(F35,FIND("(",F35)+1,FIND(")",F35)-FIND("(",F35)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="20">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1),LEN(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B36">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1),LEN(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1),LEN(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C36">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1),LEN(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1),LEN(MID(F36,FIND("(",F36)+1,FIND(")",F36)-FIND("(",F36)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="20">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F37,FIND("(",F37)+1,FIND(")",F37)-FIND("(",F37)-1),LEN(MID(F37,FIND("(",F37)+1,FIND(")",F37)-FIND("(",F37)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B37">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F37,FIND("(",F37)+1,FIND(")",F37)-FIND("(",F37)-1),LEN(MID(F37,FIND("(",F37)+1,FIND(")",F37)-FIND("(",F37)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F37,FIND("(",F37)+1,FIND(")",F37)-FIND("(",F37)-1),LEN(MID(F37,FIND("(",F37)+1,FIND(")",F37)-FIND("(",F37)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="20">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1),LEN(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B38">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1),LEN(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1),LEN(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C38">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1),LEN(MID(F38,FIND("(",F38)+1,FIND(")",F38)-FIND("(",F38)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="20">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1),LEN(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="B39">
-        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1),LEN(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1))-1,1,4),[2]Data!$B$187:$B$1389,1)),1,0)</f>
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1),LEN(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1))-1,1,5),[2]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
       <c r="C39">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1),LEN(MID(F39,FIND("(",F39)+1,FIND(")",F39)-FIND("(",F39)-1))-1,1,4),[3]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="20">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B40" t="s">
@@ -18540,12 +20017,19 @@
       <c r="C40" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="D40" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F40,FIND("(",F40)+1,FIND(")",F40)-FIND("(",F40)-1),LEN(MID(F40,FIND("(",F40)+1,FIND(")",F40)-FIND("(",F40)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="20">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B41" t="s">
@@ -18554,12 +20038,19 @@
       <c r="C41" t="s">
         <v>71</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="D41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F41,FIND("(",F41)+1,FIND(")",F41)-FIND("(",F41)-1),LEN(MID(F41,FIND("(",F41)+1,FIND(")",F41)-FIND("(",F41)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="20">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B42" t="s">
@@ -18568,12 +20059,19 @@
       <c r="C42" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="D42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F42,FIND("(",F42)+1,FIND(")",F42)-FIND("(",F42)-1),LEN(MID(F42,FIND("(",F42)+1,FIND(")",F42)-FIND("(",F42)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B43" t="s">
@@ -18582,18 +20080,19 @@
       <c r="C43" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F43" s="1" t="s">
+      <c r="E43">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F43,FIND("(",F43)+1,FIND(")",F43)-FIND("(",F43)-1),LEN(MID(F43,FIND("(",F43)+1,FIND(")",F43)-FIND("(",F43)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="20">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B44" t="s">
@@ -18602,12 +20101,19 @@
       <c r="C44" t="s">
         <v>71</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F44,FIND("(",F44)+1,FIND(")",F44)-FIND("(",F44)-1),LEN(MID(F44,FIND("(",F44)+1,FIND(")",F44)-FIND("(",F44)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="20">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B45" t="s">
@@ -18616,12 +20122,19 @@
       <c r="C45" t="s">
         <v>71</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="D45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F45,FIND("(",F45)+1,FIND(")",F45)-FIND("(",F45)-1),LEN(MID(F45,FIND("(",F45)+1,FIND(")",F45)-FIND("(",F45)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B46" t="s">
@@ -18630,12 +20143,19 @@
       <c r="C46" t="s">
         <v>71</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="D46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F46,FIND("(",F46)+1,FIND(")",F46)-FIND("(",F46)-1),LEN(MID(F46,FIND("(",F46)+1,FIND(")",F46)-FIND("(",F46)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="20">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B47" t="s">
@@ -18644,12 +20164,19 @@
       <c r="C47" t="s">
         <v>71</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="D47" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F47,FIND("(",F47)+1,FIND(")",F47)-FIND("(",F47)-1),LEN(MID(F47,FIND("(",F47)+1,FIND(")",F47)-FIND("(",F47)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="20">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B48" t="s">
@@ -18658,12 +20185,19 @@
       <c r="C48" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="D48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F48,FIND("(",F48)+1,FIND(")",F48)-FIND("(",F48)-1),LEN(MID(F48,FIND("(",F48)+1,FIND(")",F48)-FIND("(",F48)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="20">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F49,FIND("(",F49)+1,FIND(")",F49)-FIND("(",F49)-1),LEN(MID(F49,FIND("(",F49)+1,FIND(")",F49)-FIND("(",F49)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
@@ -18673,12 +20207,19 @@
       <c r="C49" t="s">
         <v>90</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="D49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F49,FIND("(",F49)+1,FIND(")",F49)-FIND("(",F49)-1),LEN(MID(F49,FIND("(",F49)+1,FIND(")",F49)-FIND("(",F49)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="20">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B50" t="s">
@@ -18687,12 +20228,19 @@
       <c r="C50" t="s">
         <v>71</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="D50" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F50,FIND("(",F50)+1,FIND(")",F50)-FIND("(",F50)-1),LEN(MID(F50,FIND("(",F50)+1,FIND(")",F50)-FIND("(",F50)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="20">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B51" t="s">
@@ -18701,12 +20249,19 @@
       <c r="C51" t="s">
         <v>92</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="D51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F51,FIND("(",F51)+1,FIND(")",F51)-FIND("(",F51)-1),LEN(MID(F51,FIND("(",F51)+1,FIND(")",F51)-FIND("(",F51)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B52" t="s">
@@ -18715,12 +20270,19 @@
       <c r="C52" t="s">
         <v>71</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="D52" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F52,FIND("(",F52)+1,FIND(")",F52)-FIND("(",F52)-1),LEN(MID(F52,FIND("(",F52)+1,FIND(")",F52)-FIND("(",F52)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="20">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B53" t="s">
@@ -18729,12 +20291,19 @@
       <c r="C53" t="s">
         <v>71</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="D53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F53,FIND("(",F53)+1,FIND(")",F53)-FIND("(",F53)-1),LEN(MID(F53,FIND("(",F53)+1,FIND(")",F53)-FIND("(",F53)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="20">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B54" t="s">
@@ -18743,12 +20312,19 @@
       <c r="C54" t="s">
         <v>71</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="D54" t="s">
+        <v>71</v>
+      </c>
+      <c r="E54">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F54,FIND("(",F54)+1,FIND(")",F54)-FIND("(",F54)-1),LEN(MID(F54,FIND("(",F54)+1,FIND(")",F54)-FIND("(",F54)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B55" t="s">
@@ -18757,12 +20333,19 @@
       <c r="C55" t="s">
         <v>71</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="D55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F55,FIND("(",F55)+1,FIND(")",F55)-FIND("(",F55)-1),LEN(MID(F55,FIND("(",F55)+1,FIND(")",F55)-FIND("(",F55)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="20">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B56" t="s">
@@ -18771,12 +20354,19 @@
       <c r="C56" t="s">
         <v>71</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="D56" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F56,FIND("(",F56)+1,FIND(")",F56)-FIND("(",F56)-1),LEN(MID(F56,FIND("(",F56)+1,FIND(")",F56)-FIND("(",F56)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="20">
-      <c r="A57" s="2">
+      <c r="A57" s="1">
         <f>IF(ISNUMBER(MATCH(REPLACE(MID(F57,FIND("(",F57)+1,FIND(")",F57)-FIND("(",F57)-1),LEN(MID(F57,FIND("(",F57)+1,FIND(")",F57)-FIND("(",F57)-1))-1,1,4),[1]Data!$B$187:$B$1389,1)),1,0)</f>
         <v>1</v>
       </c>
@@ -18786,12 +20376,19 @@
       <c r="C57" t="s">
         <v>91</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="D57" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F57,FIND("(",F57)+1,FIND(")",F57)-FIND("(",F57)-1),LEN(MID(F57,FIND("(",F57)+1,FIND(")",F57)-FIND("(",F57)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B58" t="s">
@@ -18800,12 +20397,19 @@
       <c r="C58" t="s">
         <v>71</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="D58" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F58,FIND("(",F58)+1,FIND(")",F58)-FIND("(",F58)-1),LEN(MID(F58,FIND("(",F58)+1,FIND(")",F58)-FIND("(",F58)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="20">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B59" t="s">
@@ -18814,12 +20418,19 @@
       <c r="C59" t="s">
         <v>93</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="D59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E59">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F59,FIND("(",F59)+1,FIND(")",F59)-FIND("(",F59)-1),LEN(MID(F59,FIND("(",F59)+1,FIND(")",F59)-FIND("(",F59)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="20">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B60" t="s">
@@ -18828,12 +20439,19 @@
       <c r="C60" t="s">
         <v>71</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="D60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F60,FIND("(",F60)+1,FIND(")",F60)-FIND("(",F60)-1),LEN(MID(F60,FIND("(",F60)+1,FIND(")",F60)-FIND("(",F60)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="20">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B61" t="s">
@@ -18842,12 +20460,19 @@
       <c r="C61" t="s">
         <v>71</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="D61" t="s">
+        <v>71</v>
+      </c>
+      <c r="E61">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F61,FIND("(",F61)+1,FIND(")",F61)-FIND("(",F61)-1),LEN(MID(F61,FIND("(",F61)+1,FIND(")",F61)-FIND("(",F61)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="20">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B62" t="s">
@@ -18856,12 +20481,19 @@
       <c r="C62" t="s">
         <v>71</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="D62" t="s">
+        <v>71</v>
+      </c>
+      <c r="E62">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F62,FIND("(",F62)+1,FIND(")",F62)-FIND("(",F62)-1),LEN(MID(F62,FIND("(",F62)+1,FIND(")",F62)-FIND("(",F62)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="20">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B63" t="s">
@@ -18870,12 +20502,19 @@
       <c r="C63" t="s">
         <v>71</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="D63" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F63,FIND("(",F63)+1,FIND(")",F63)-FIND("(",F63)-1),LEN(MID(F63,FIND("(",F63)+1,FIND(")",F63)-FIND("(",F63)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="20">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B64" t="s">
@@ -18884,33 +20523,76 @@
       <c r="C64" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="D64" t="s">
+        <v>71</v>
+      </c>
+      <c r="E64">
+        <f>IF(ISNUMBER(MATCH(REPLACE(MID(F64,FIND("(",F64)+1,FIND(")",F64)-FIND("(",F64)-1),LEN(MID(F64,FIND("(",F64)+1,FIND(")",F64)-FIND("(",F64)-1))-1,1,9),[4]SCRIP90_data1!$B$187:$B$401,1)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="3:3">
+    <row r="67" spans="3:6">
       <c r="C67" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="3:3">
-      <c r="C68" s="3" t="s">
+    <row r="68" spans="3:6">
+      <c r="C68" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="D68" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F68" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="69" spans="3:3">
-      <c r="C69" s="3" t="s">
+    <row r="69" spans="3:6">
+      <c r="C69" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="D69" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F69" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="70" spans="3:3">
-      <c r="C70" s="3" t="s">
+    <row r="70" spans="3:6">
+      <c r="C70" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="D70" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F70" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="71" spans="3:3">
-      <c r="C71" s="3" t="s">
+    <row r="71" spans="3:6">
+      <c r="C71" s="2" t="s">
         <v>82</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F71" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>